<commit_message>
adder three wisher text files
</commit_message>
<xml_diff>
--- a/BirthDay Wisher/people.xlsx
+++ b/BirthDay Wisher/people.xlsx
@@ -270,7 +270,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,7 +315,7 @@
       <c r="A4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="0" t="s">
@@ -326,6 +326,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="kishorelesnar77@gmail.com"/>
     <hyperlink ref="B3" r:id="rId2" display="kishorekishy77@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="kishoreravichandran7714@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>